<commit_message>
Aggiornamento del tracciato Excel in seguito a correzione refusi
</commit_message>
<xml_diff>
--- a/Semplificato2021/TracciatoXLSX/XLSX_TIS_SEMPLIFICATO_2021.xlsx
+++ b/Semplificato2021/TracciatoXLSX/XLSX_TIS_SEMPLIFICATO_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://formatemp-my.sharepoint.com/personal/dconte_formatemp_onmicrosoft_com/Documents/FTWEB/TIS SEMPLIFICATO/CIRCOLARE DEFINITIVA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarioConte\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{22DBD788-485E-AF4E-B389-A82FF4CF83EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7787F98-D301-481F-BB8E-F9211069405C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC528B5-4927-4E13-AC87-E0C82AE7F65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="483" xr2:uid="{C62F197E-4834-1546-9B8C-4BDFB4210C62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="483" activeTab="1" xr2:uid="{C62F197E-4834-1546-9B8C-4BDFB4210C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Istanze" sheetId="1" r:id="rId1"/>
@@ -754,27 +754,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7CC479-9EB7-1D4B-A1C1-E99C9EBFB207}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="27.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="27.8984375" style="2" customWidth="1"/>
     <col min="4" max="5" width="23" style="4" customWidth="1"/>
     <col min="6" max="6" width="25" style="2" customWidth="1"/>
     <col min="7" max="7" width="22" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="24.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.09765625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="2"/>
     <col min="12" max="12" width="22" style="2" customWidth="1"/>
-    <col min="13" max="13" width="24.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="24.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.59765625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +818,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -859,7 +859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -900,7 +900,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
@@ -1021,42 +1021,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2A5F62-5E65-EE42-A866-6CDFA1827C3F}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.09765625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="41.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="38.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="37" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="36.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="37.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="34.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="37.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.69921875" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="32.5" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="34.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="AB1" s="3"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9b7z8A0Rv6Q2GjcWhCMytkWwfStZrcFB4Xcv2YaZYVSweRfoDV55d2AKvLnTVq8Q/D1bZ8jhyscKZRhl6KSl4w==" saltValue="YGZagmB7tflph+ayOhYKUA==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="r+HGiC7sgWftfkZhzg3Y4x5MFeSh8zuZcXzcfZUAMm0aCud050jjMa4rpt6eqUQeTSFh4L4lfLIgK7HUM4897g==" saltValue="ZOfRJYc6Uo1FwkCjcMUg5g==" spinCount="100000" sheet="1" selectLockedCells="1" autoFilter="0"/>
   <autoFilter ref="A1:V1" xr:uid="{B1E0D013-8FDE-4AA2-A0C8-EA9D2E0E0052}"/>
   <dataConsolidate/>
   <dataValidations count="17">
@@ -1546,25 +1546,25 @@
           </x14:formula1>
           <xm:sqref>J6:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 23/03/2021" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 12 luglio:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 23/03/2021" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 12 luglio:_x000a_S = SI_x000a_N = NO" xr:uid="{FDB633D4-DFA5-490F-BD04-9DF315E6E673}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 23/03/2021" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 23 marzo 2021:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 23/03/2021" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 23 marzo 2021:_x000a_S = SI_x000a_N = NO" xr:uid="{FDB633D4-DFA5-490F-BD04-9DF315E6E673}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>U2:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 22/10/2021" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 9 novembre:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 22/10/2021" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 9 novembre:_x000a_S = SI_x000a_N = NO" xr:uid="{5E5A4C24-76B1-4D01-B954-B2FF3213F404}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 22/10/2021" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 22 ottobre 2021:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 22/10/2021" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 22 ottobre 2021:_x000a_S = SI_x000a_N = NO" xr:uid="{5E5A4C24-76B1-4D01-B954-B2FF3213F404}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>V2:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 04/01/2021" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 04/01/2021" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO" xr:uid="{D12F55EB-BC54-46B9-B63F-1B0D244EC976}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 04/01/2021" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 4 gennaio 2021:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 04/01/2021" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 4 gennaio 2021:_x000a_S = SI_x000a_N = NO" xr:uid="{D12F55EB-BC54-46B9-B63F-1B0D244EC976}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>T2:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 9/11/2020" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 9/11/2020" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 25 marzo:_x000a_S = SI_x000a_N = NO" xr:uid="{804DA3F7-D42F-45D1-8DAC-A2CB09DBDC59}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lavoratore Dip 9/11/2020" error="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 9 novembre 2020:_x000a_S = SI_x000a_N = NO" promptTitle="Lavoratore Dip 9/11/2020" prompt="Inserire se il lavoratore è alle dipendenze dell'agenzia alla data del 9 novembre 2020:_x000a_S = SI_x000a_N = NO" xr:uid="{804DA3F7-D42F-45D1-8DAC-A2CB09DBDC59}">
           <x14:formula1>
             <xm:f>Tipologiche!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1587,17 +1587,17 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
     <col min="3" max="4" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1619,13 +1619,13 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1633,13 +1633,13 @@
         <v>20</v>
       </c>
       <c r="C3" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1647,13 +1647,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1661,13 +1661,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -1675,13 +1675,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -1689,13 +1689,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -1703,13 +1703,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -1717,13 +1717,13 @@
         <v>18</v>
       </c>
       <c r="C9" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -1731,13 +1731,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D10" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1745,13 +1745,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D11" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1759,13 +1759,13 @@
         <v>20</v>
       </c>
       <c r="C12" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D12" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1773,13 +1773,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D13" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1787,13 +1787,13 @@
         <v>14</v>
       </c>
       <c r="C14" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D14" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
@@ -1801,13 +1801,13 @@
         <v>15</v>
       </c>
       <c r="C15" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D15" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1815,13 +1815,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D16" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -1829,13 +1829,13 @@
         <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D17" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -1843,13 +1843,13 @@
         <v>18</v>
       </c>
       <c r="C18" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D18" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1857,18 +1857,18 @@
         <v>8</v>
       </c>
       <c r="C19" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D19" s="2">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GCbIAsr8eS4O/CdNCrYvx2AKQspNRh2QrQ7GDupUPm8CRqmb8TL7gNqcNEIN9GIyaXtMJxDzi4kfLrKV1iaOGg==" saltValue="XhiDTMg0p31FHsvJtMDjXQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="deqXLCDP+A1omzmEfeimWHGQLRF92Hsxtmhy7dTtNKwt8icZBW9q9fXxCR5v861tRoIoWpnZnZghNRGwBphCuw==" saltValue="1NSIvMNm97ME5EGkYph3sg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Anno riferimento " error="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2020)" promptTitle="Anno riferimento " prompt="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2020)" sqref="C2:C1048576" xr:uid="{7D64DC23-DD90-4842-A22A-F55D04ACAC42}">
-      <formula1>2020</formula1>
+    <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Anno riferimento " error="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2021)" promptTitle="Anno riferimento " prompt="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2021)" sqref="C2:C1048576" xr:uid="{7D64DC23-DD90-4842-A22A-F55D04ACAC42}">
+      <formula1>2021</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mese Riferimento" error="Inserire il mese a cui fa riferimento il numero di giornate fruite indicate (2-12)" promptTitle="Mese Riferimento" prompt="Inserire il mese a cui fa riferimento il numero di giornate fruite indicate (valori ammessi da 2 a 12)" sqref="D2:D1048576" xr:uid="{43C46FAE-6C02-44EF-80A5-F4645E052DB5}">
       <formula1>2</formula1>
@@ -1899,18 +1899,18 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.3984375" style="2" customWidth="1"/>
     <col min="4" max="12" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="22.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="18" width="22.09765625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -2004,7 +2004,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>44232</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>44370</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D7" s="5"/>
     </row>
   </sheetData>
@@ -2102,12 +2102,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>40</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Sostituzione tracciato (sistemato foglio giornate fruite)
</commit_message>
<xml_diff>
--- a/Semplificato2021/TracciatoXLSX/XLSX_TIS_SEMPLIFICATO_2021.xlsx
+++ b/Semplificato2021/TracciatoXLSX/XLSX_TIS_SEMPLIFICATO_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarioConte\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarioConte\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC528B5-4927-4E13-AC87-E0C82AE7F65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A464CD1-7F92-49F4-B263-A2DDF0739EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="483" activeTab="1" xr2:uid="{C62F197E-4834-1546-9B8C-4BDFB4210C62}"/>
+    <workbookView xWindow="28680" yWindow="165" windowWidth="29040" windowHeight="15990" tabRatio="483" activeTab="2" xr2:uid="{C62F197E-4834-1546-9B8C-4BDFB4210C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Istanze" sheetId="1" r:id="rId1"/>
@@ -1021,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2A5F62-5E65-EE42-A866-6CDFA1827C3F}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861E526C-F842-4CA2-AE86-3C3CCBFAC172}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1864,14 +1864,14 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="deqXLCDP+A1omzmEfeimWHGQLRF92Hsxtmhy7dTtNKwt8icZBW9q9fXxCR5v861tRoIoWpnZnZghNRGwBphCuw==" saltValue="1NSIvMNm97ME5EGkYph3sg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mX/Gii/TvmevSXZQX4EMVCS6jL+xXYPvQmdI2udHIXrJ21zWDcGSwIRUef0slc2I+d+Uf25YiBD7zC45LKPoyg==" saltValue="pLm0tJNrN5QpC3wp25f0Ew==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <dataValidations count="3">
     <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Anno riferimento " error="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2021)" promptTitle="Anno riferimento " prompt="Inserire l'anno di riferimento di cui si stanno indicate le giornate fruite (fisso 2021)" sqref="C2:C1048576" xr:uid="{7D64DC23-DD90-4842-A22A-F55D04ACAC42}">
       <formula1>2021</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mese Riferimento" error="Inserire il mese a cui fa riferimento il numero di giornate fruite indicate (2-12)" promptTitle="Mese Riferimento" prompt="Inserire il mese a cui fa riferimento il numero di giornate fruite indicate (valori ammessi da 2 a 12)" sqref="D2:D1048576" xr:uid="{43C46FAE-6C02-44EF-80A5-F4645E052DB5}">
-      <formula1>2</formula1>
+      <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
     <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Errore inserimento" error="Indicare il numero totale delle giornate fruite per il mese a cui fa riferimento (colonna D, mese) - max 31" promptTitle="Totale Giornate Fruite" prompt="Indicare il numero totale delle giornate fruite per il mese a cui fa riferimento (colonna D, mese) - max 31" sqref="B2:B1048576" xr:uid="{49B50356-0908-4079-B049-A5C2B3891F8B}">
@@ -1879,6 +1879,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>